<commit_message>
Formulas are reliably evaluated and wordwrap and test cleanup
</commit_message>
<xml_diff>
--- a/EmailHandling/EmailConcatenationPOC/EmailConcatenationPOC/Excel/workbook_calcs.xlsx
+++ b/EmailHandling/EmailConcatenationPOC/EmailConcatenationPOC/Excel/workbook_calcs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hooverrl\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hooverrl\Desktop\NCI\nciitrc_eGrants\EmailHandling\EmailConcatenationPOC\EmailConcatenationPOC\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAF42887-792D-46E2-9FA9-B66EC0C83E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB8073C-6EF8-47C5-9601-F5E553730F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" xr2:uid="{2681E5C2-0459-482F-B7AB-22E9BF1D43B0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2681E5C2-0459-482F-B7AB-22E9BF1D43B0}"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>lorem</t>
   </si>
@@ -135,13 +135,16 @@
     <t>thousand separator</t>
   </si>
   <si>
-    <t>XSLX</t>
-  </si>
-  <si>
     <t>Sum :</t>
   </si>
   <si>
     <t>Total :</t>
+  </si>
+  <si>
+    <t>here is some lorem ipsum supporting what should appear as a word wrap. It should NOT be one very long cell.</t>
+  </si>
+  <si>
+    <t>XLSX</t>
   </si>
 </sst>
 </file>
@@ -298,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -325,6 +328,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -661,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7312F71-4FBC-4C7B-865C-2F002FB94AC7}">
   <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +683,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -736,17 +742,20 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="90" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>16</v>
       </c>
+      <c r="F15" s="20" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -760,7 +769,7 @@
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19">
         <f>SUM(C17:C18)</f>

</xml_diff>